<commit_message>
css plus ou moins fini pour creerSalle
</commit_message>
<xml_diff>
--- a/C61/sprint0/Planification.xlsx
+++ b/C61/sprint0/Planification.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F460934-9970-42DE-9F23-83952CB07AF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC84E1ED-049B-4892-9E02-DCDF864A45C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{087A1B5B-7B97-4327-AC94-7D0ECF997B43}"/>
   </bookViews>
@@ -483,7 +483,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -499,6 +499,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF9F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -747,7 +753,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -828,16 +834,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -846,7 +843,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -858,7 +855,22 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3213,8 +3225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDA4BA3A-0DAF-4F83-AB3B-26EE796DD82A}">
   <dimension ref="C3:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32:D33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36:D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3246,279 +3258,279 @@
       <c r="D7" s="46"/>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="50" t="s">
+      <c r="C8" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="53" t="s">
+      <c r="D8" s="50" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="9" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="49"/>
-      <c r="D9" s="54"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="56"/>
     </row>
     <row r="10" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="50" t="s">
+      <c r="D10" s="48" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="11" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="49"/>
-      <c r="D11" s="51"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="55"/>
     </row>
     <row r="12" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="53" t="s">
+      <c r="D12" s="50" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="13" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="49"/>
-      <c r="D13" s="54"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="56"/>
     </row>
     <row r="14" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C14" s="50" t="s">
+      <c r="C14" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="50" t="s">
+      <c r="D14" s="48" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="15" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="52"/>
-      <c r="D15" s="51"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="55"/>
     </row>
     <row r="16" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C16" s="50" t="s">
+      <c r="C16" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="53" t="s">
+      <c r="D16" s="50" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="17" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="52"/>
-      <c r="D17" s="54"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="56"/>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C18" s="50" t="s">
+      <c r="C18" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="50" t="s">
+      <c r="D18" s="48" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="19" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="52"/>
-      <c r="D19" s="51"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="55"/>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20" s="50" t="s">
+      <c r="C20" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="53" t="s">
+      <c r="D20" s="50" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="21" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="52"/>
-      <c r="D21" s="54"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="56"/>
     </row>
     <row r="22" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="50" t="s">
+      <c r="C22" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="50" t="s">
+      <c r="D22" s="48" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="23" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="55"/>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C24" s="50" t="s">
+      <c r="C24" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="50" t="s">
+      <c r="D24" s="48" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="25" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="52"/>
-      <c r="D25" s="51"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="55"/>
     </row>
     <row r="26" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="50" t="s">
+      <c r="C26" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="D26" s="53" t="s">
+      <c r="D26" s="50" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="27" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="52"/>
-      <c r="D27" s="54"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="56"/>
     </row>
     <row r="28" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="50" t="s">
+      <c r="C28" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="50" t="s">
+      <c r="D28" s="48" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="29" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="52"/>
-      <c r="D29" s="52"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
     </row>
     <row r="30" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="50" t="s">
+      <c r="C30" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="50" t="s">
+      <c r="D30" s="48" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="31" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C31" s="52"/>
-      <c r="D31" s="51"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="55"/>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C32" s="50" t="s">
+      <c r="C32" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="D32" s="50" t="s">
+      <c r="D32" s="48" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="33" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="52"/>
-      <c r="D33" s="51"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="55"/>
     </row>
     <row r="34" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="50" t="s">
+      <c r="C34" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="50" t="s">
+      <c r="D34" s="48" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="35" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C35" s="52"/>
-      <c r="D35" s="51"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="55"/>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C36" s="50" t="s">
+      <c r="C36" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="D36" s="55" t="s">
+      <c r="D36" s="59" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="37" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="52"/>
-      <c r="D37" s="56"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="60"/>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C38" s="50" t="s">
+      <c r="C38" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="55" t="s">
+      <c r="D38" s="52" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="39" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C39" s="52"/>
-      <c r="D39" s="56"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="53"/>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C40" s="50" t="s">
+      <c r="C40" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="D40" s="55" t="s">
+      <c r="D40" s="52" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="41" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="52"/>
-      <c r="D41" s="57"/>
+      <c r="C41" s="49"/>
+      <c r="D41" s="54"/>
     </row>
     <row r="42" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C42" s="50" t="s">
+      <c r="C42" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="D42" s="53" t="s">
+      <c r="D42" s="50" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="43" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C43" s="52"/>
-      <c r="D43" s="58"/>
+      <c r="C43" s="49"/>
+      <c r="D43" s="51"/>
     </row>
     <row r="44" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C44" s="50"/>
-      <c r="D44" s="50"/>
+      <c r="C44" s="48"/>
+      <c r="D44" s="48"/>
     </row>
     <row r="45" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C45" s="52"/>
-      <c r="D45" s="52"/>
+      <c r="C45" s="49"/>
+      <c r="D45" s="49"/>
     </row>
     <row r="46" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C46" s="50"/>
-      <c r="D46" s="50"/>
+      <c r="C46" s="48"/>
+      <c r="D46" s="48"/>
     </row>
     <row r="47" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C47" s="52"/>
-      <c r="D47" s="52"/>
+      <c r="C47" s="49"/>
+      <c r="D47" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:D41"/>
     <mergeCell ref="C42:C43"/>
     <mergeCell ref="D42:D43"/>
     <mergeCell ref="C44:C45"/>
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="C46:C47"/>
     <mergeCell ref="D46:D47"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C18:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajout des fonctionnalités faites dans le sprint 1
</commit_message>
<xml_diff>
--- a/C61/sprint0/Planification.xlsx
+++ b/C61/sprint0/Planification.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC84E1ED-049B-4892-9E02-DCDF864A45C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D9BB5F-C773-4E94-A5C8-D0904849DBCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{087A1B5B-7B97-4327-AC94-7D0ECF997B43}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{087A1B5B-7B97-4327-AC94-7D0ECF997B43}"/>
   </bookViews>
   <sheets>
     <sheet name="Tâche" sheetId="1" r:id="rId1"/>
@@ -483,7 +483,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -505,6 +505,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -753,7 +759,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -840,10 +846,25 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -855,22 +876,13 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3226,7 +3238,7 @@
   <dimension ref="C3:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36:D37"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3261,121 +3273,121 @@
       <c r="C8" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="50" t="s">
+      <c r="D8" s="53" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="9" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="57"/>
-      <c r="D9" s="56"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="54"/>
     </row>
     <row r="10" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="58" t="s">
+      <c r="C10" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="48" t="s">
+      <c r="D10" s="53" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="11" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="57"/>
-      <c r="D11" s="55"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="54"/>
     </row>
     <row r="12" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="58" t="s">
+      <c r="C12" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="50" t="s">
+      <c r="D12" s="53" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="13" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="57"/>
-      <c r="D13" s="56"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="54"/>
     </row>
     <row r="14" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C14" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="48" t="s">
+      <c r="D14" s="53" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="15" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="49"/>
-      <c r="D15" s="55"/>
+      <c r="D15" s="54"/>
     </row>
     <row r="16" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C16" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="50" t="s">
+      <c r="D16" s="53" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="17" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="49"/>
-      <c r="D17" s="56"/>
+      <c r="D17" s="54"/>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C18" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="48" t="s">
+      <c r="D18" s="53" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="19" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C19" s="49"/>
-      <c r="D19" s="55"/>
+      <c r="D19" s="54"/>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C20" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="50" t="s">
+      <c r="D20" s="53" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="21" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="49"/>
-      <c r="D21" s="56"/>
+      <c r="D21" s="54"/>
     </row>
     <row r="22" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="48" t="s">
+      <c r="D22" s="53" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="23" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="55"/>
-      <c r="D23" s="55"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="54"/>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C24" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="48" t="s">
+      <c r="D24" s="61" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="25" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C25" s="49"/>
-      <c r="D25" s="55"/>
+      <c r="D25" s="62"/>
     </row>
     <row r="26" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="D26" s="50" t="s">
+      <c r="D26" s="53" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="27" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="49"/>
-      <c r="D27" s="56"/>
+      <c r="D27" s="54"/>
     </row>
     <row r="28" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" s="48" t="s">
@@ -3393,13 +3405,13 @@
       <c r="C30" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="48" t="s">
+      <c r="D30" s="61" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="31" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="49"/>
-      <c r="D31" s="55"/>
+      <c r="D31" s="62"/>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C32" s="48" t="s">
@@ -3411,67 +3423,67 @@
     </row>
     <row r="33" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="49"/>
-      <c r="D33" s="55"/>
+      <c r="D33" s="52"/>
     </row>
     <row r="34" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C34" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="48" t="s">
+      <c r="D34" s="61" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="35" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="49"/>
-      <c r="D35" s="55"/>
+      <c r="D35" s="62"/>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C36" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="D36" s="59" t="s">
+      <c r="D36" s="55" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="37" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="49"/>
-      <c r="D37" s="60"/>
+      <c r="D37" s="56"/>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C38" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="52" t="s">
+      <c r="D38" s="57" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="39" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="49"/>
-      <c r="D39" s="53"/>
+      <c r="D39" s="58"/>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C40" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="D40" s="52" t="s">
+      <c r="D40" s="57" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="41" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C41" s="49"/>
-      <c r="D41" s="54"/>
+      <c r="D41" s="59"/>
     </row>
     <row r="42" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C42" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="D42" s="50" t="s">
+      <c r="D42" s="53" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="43" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" s="49"/>
-      <c r="D43" s="51"/>
+      <c r="D43" s="60"/>
     </row>
     <row r="44" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C44" s="48"/>
@@ -3491,46 +3503,46 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D16:D17"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D16:D17"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="D22:D23"/>
     <mergeCell ref="D24:D25"/>
     <mergeCell ref="D26:D27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C16:C17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>